<commit_message>
New RU Localization files
</commit_message>
<xml_diff>
--- a/CustomLocalization/Localization/RogueTech/RU/MechEngineer/LocalizationDef.xlsx
+++ b/CustomLocalization/Localization/RogueTech/RU/MechEngineer/LocalizationDef.xlsx
@@ -4150,7 +4150,7 @@
     <t>{0} Inc.Sensor Range</t>
   </si>
   <si>
-    <t>{0}+100% дальность работы сенсоров</t>
+    <t>{0} дальность работы сенсоров</t>
   </si>
   <si>
     <t>MechEngineer.ActiveSight.Long</t>
@@ -14449,7 +14449,7 @@
     <t>Increases Maximum Carry Weight by {0}</t>
   </si>
   <si>
-    <t>Увеличивает максимальную полезную нагрузку на {0}</t>
+    <t>Увеличивает грузоподъемность спец. слотов на {0}</t>
   </si>
   <si>
     <t>MechEngineer.CarryCapacityExplain.Full</t>
@@ -21957,8 +21957,8 @@
   <dimension ref="A1:D4031"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3937" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3954" sqref="C3954"/>
+      <pane ySplit="1" topLeftCell="A1970" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1996" sqref="C1996"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -28189,7 +28189,7 @@
       <c r="B566" s="16" t="s">
         <v>1376</v>
       </c>
-      <c r="C566" s="39" t="s">
+      <c r="C566" s="50" t="s">
         <v>1377</v>
       </c>
     </row>
@@ -31005,7 +31005,7 @@
       <c r="B822" s="16" t="s">
         <v>1376</v>
       </c>
-      <c r="C822" s="39" t="s">
+      <c r="C822" s="50" t="s">
         <v>1377</v>
       </c>
     </row>
@@ -31148,7 +31148,7 @@
       <c r="B835" s="16" t="s">
         <v>1376</v>
       </c>
-      <c r="C835" s="39" t="s">
+      <c r="C835" s="50" t="s">
         <v>1377</v>
       </c>
     </row>
@@ -31170,7 +31170,7 @@
       <c r="B837" s="16" t="s">
         <v>1376</v>
       </c>
-      <c r="C837" s="39" t="s">
+      <c r="C837" s="50" t="s">
         <v>1377</v>
       </c>
     </row>
@@ -31192,7 +31192,7 @@
       <c r="B839" s="16" t="s">
         <v>1376</v>
       </c>
-      <c r="C839" s="39" t="s">
+      <c r="C839" s="50" t="s">
         <v>1377</v>
       </c>
     </row>
@@ -31929,7 +31929,7 @@
       <c r="B906" s="16" t="s">
         <v>2147</v>
       </c>
-      <c r="C906" s="39" t="s">
+      <c r="C906" s="50" t="s">
         <v>1377</v>
       </c>
     </row>
@@ -43765,7 +43765,7 @@
       <c r="B1982" s="16" t="s">
         <v>4770</v>
       </c>
-      <c r="C1982" s="6" t="s">
+      <c r="C1982" s="41" t="s">
         <v>4771</v>
       </c>
     </row>
@@ -43905,10 +43905,10 @@
       <c r="A1995" s="13" t="s">
         <v>4808</v>
       </c>
-      <c r="B1995" s="16" t="s">
+      <c r="B1995" s="50" t="s">
         <v>4809</v>
       </c>
-      <c r="C1995" s="16" t="s">
+      <c r="C1995" s="49" t="s">
         <v>4810</v>
       </c>
     </row>

</xml_diff>